<commit_message>
Add: pipes & blockQ & level1 map
</commit_message>
<xml_diff>
--- a/coordinate.xlsx
+++ b/coordinate.xlsx
@@ -1,19 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19126"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19226"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\OOP_SuperAdventure\測試\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4F82ECBE-B1A5-4A67-8CEE-B43A358583E3}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{226584F1-A705-43EA-BB9E-6376DF3C6C1D}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="10296" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16200" windowHeight="5592" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="工作表1" sheetId="1" r:id="rId1"/>
+    <sheet name="工作表2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="179017" concurrentCalc="0"/>
   <extLst>
@@ -28,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="25">
   <si>
     <t>gournd_x</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -103,6 +104,30 @@
   </si>
   <si>
     <t>{x: 1220, y: 450},</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>block width</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Bridge{x, y}</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ground{x, y}</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>blockQ{x,y}</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>{x:490, y: 570}</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>stage{x, y}</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -429,10 +454,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H59"/>
+  <dimension ref="A1:L67"/>
   <sheetViews>
-    <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
-      <selection activeCell="H12" sqref="H12:H14"/>
+    <sheetView showRuler="0" workbookViewId="0">
+      <selection activeCell="C1" sqref="C1:C1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="16.2" x14ac:dyDescent="0.3"/>
@@ -442,7 +467,7 @@
     <col min="8" max="8" width="17.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -450,7 +475,133 @@
         <v>780</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="J2">
+        <f>I2</f>
+        <v>0</v>
+      </c>
+      <c r="K2">
+        <f t="shared" ref="K2:L2" si="0">J2</f>
+        <v>0</v>
+      </c>
+      <c r="L2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="J3">
+        <f>$I3</f>
+        <v>0</v>
+      </c>
+      <c r="K3">
+        <f t="shared" ref="K3:L3" si="1">$I3</f>
+        <v>0</v>
+      </c>
+      <c r="L3">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="J4">
+        <f t="shared" ref="J4:J12" si="2">I4</f>
+        <v>0</v>
+      </c>
+      <c r="K4">
+        <f t="shared" ref="K4:L4" si="3">J4</f>
+        <v>0</v>
+      </c>
+      <c r="L4">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="J5">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="K5">
+        <f t="shared" ref="K5:L5" si="4">J5</f>
+        <v>0</v>
+      </c>
+      <c r="L5">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="J6">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="K6">
+        <f t="shared" ref="K6:L6" si="5">J6</f>
+        <v>0</v>
+      </c>
+      <c r="L6">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="J7">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="K7">
+        <f t="shared" ref="K7:L7" si="6">J7</f>
+        <v>0</v>
+      </c>
+      <c r="L7">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="J8">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="K8">
+        <f t="shared" ref="K8:L8" si="7">J8</f>
+        <v>0</v>
+      </c>
+      <c r="L8">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="J9">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="K9">
+        <f t="shared" ref="K9:L9" si="8">J9</f>
+        <v>0</v>
+      </c>
+      <c r="L9">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="J10">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="K10">
+        <f t="shared" ref="K10:L10" si="9">J10</f>
+        <v>0</v>
+      </c>
+      <c r="L10">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>1</v>
       </c>
@@ -466,10 +617,22 @@
       <c r="H11" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="J11">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="K11">
+        <f t="shared" ref="K11:L11" si="10">J11</f>
+        <v>0</v>
+      </c>
+      <c r="L11">
+        <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A12" t="str">
-        <f t="shared" ref="A12:A27" si="0">"{x: "&amp;30+$B12&amp;", y: "&amp;$B$1&amp;"},"</f>
+        <f>"{x: " &amp; 30+$B12&amp;", y: "&amp;$B$1&amp;"},"</f>
         <v>{x: 30, y: 780},</v>
       </c>
       <c r="B12">
@@ -485,17 +648,29 @@
       <c r="H12" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="J12">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="K12">
+        <f t="shared" ref="K12:L12" si="11">J12</f>
+        <v>0</v>
+      </c>
+      <c r="L12">
+        <f t="shared" si="11"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A13" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" ref="A13:A27" si="12">"{x: "&amp;30+$B13&amp;", y: "&amp;$B$1&amp;"},"</f>
         <v>{x: 100, y: 780},</v>
       </c>
       <c r="B13">
         <v>70</v>
       </c>
       <c r="E13" t="str">
-        <f t="shared" ref="E13:E24" si="1">"{x: "&amp;30&amp;", y: "&amp;710-F13&amp;"},"</f>
+        <f t="shared" ref="E13:E24" si="13">"{x: "&amp;30&amp;", y: "&amp;710-F13&amp;"},"</f>
         <v>{x: 30, y: 640},</v>
       </c>
       <c r="F13">
@@ -504,17 +679,21 @@
       <c r="H13" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="J13">
+        <f t="shared" ref="J13" si="14">I13</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A14" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="12"/>
         <v>{x: 170, y: 780},</v>
       </c>
       <c r="B14">
         <v>140</v>
       </c>
       <c r="E14" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="13"/>
         <v>{x: 30, y: 570},</v>
       </c>
       <c r="F14">
@@ -523,49 +702,61 @@
       <c r="H14" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="J14">
+        <f t="shared" ref="J14" si="15">I14</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A15" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="12"/>
         <v>{x: 240, y: 780},</v>
       </c>
       <c r="B15">
         <v>210</v>
       </c>
       <c r="E15" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="13"/>
         <v>{x: 30, y: 500},</v>
       </c>
       <c r="F15">
         <v>210</v>
       </c>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="J15">
+        <f t="shared" ref="J15" si="16">I15</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A16" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="12"/>
         <v>{x: 310, y: 780},</v>
       </c>
       <c r="B16">
         <v>280</v>
       </c>
       <c r="E16" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="13"/>
         <v>{x: 30, y: 430},</v>
       </c>
       <c r="F16">
         <v>280</v>
       </c>
+      <c r="J16">
+        <f t="shared" ref="J16" si="17">I16</f>
+        <v>0</v>
+      </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A17" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="12"/>
         <v>{x: 380, y: 780},</v>
       </c>
       <c r="B17">
         <v>350</v>
       </c>
       <c r="E17" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="13"/>
         <v>{x: 30, y: 360},</v>
       </c>
       <c r="F17">
@@ -574,14 +765,14 @@
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A18" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="12"/>
         <v>{x: 450, y: 780},</v>
       </c>
       <c r="B18">
         <v>420</v>
       </c>
       <c r="E18" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="13"/>
         <v>{x: 30, y: 290},</v>
       </c>
       <c r="F18">
@@ -590,14 +781,14 @@
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A19" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="12"/>
         <v>{x: 520, y: 780},</v>
       </c>
       <c r="B19">
         <v>490</v>
       </c>
       <c r="E19" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="13"/>
         <v>{x: 30, y: 220},</v>
       </c>
       <c r="F19">
@@ -606,14 +797,14 @@
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A20" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="12"/>
         <v>{x: 590, y: 780},</v>
       </c>
       <c r="B20">
         <v>560</v>
       </c>
       <c r="E20" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="13"/>
         <v>{x: 30, y: 150},</v>
       </c>
       <c r="F20">
@@ -622,14 +813,14 @@
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A21" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="12"/>
         <v>{x: 660, y: 780},</v>
       </c>
       <c r="B21">
         <v>630</v>
       </c>
       <c r="E21" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="13"/>
         <v>{x: 30, y: 80},</v>
       </c>
       <c r="F21">
@@ -638,14 +829,14 @@
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A22" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="12"/>
         <v>{x: 730, y: 780},</v>
       </c>
       <c r="B22">
         <v>700</v>
       </c>
       <c r="E22" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="13"/>
         <v>{x: 30, y: 10},</v>
       </c>
       <c r="F22">
@@ -654,14 +845,14 @@
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A23" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="12"/>
         <v>{x: 800, y: 780},</v>
       </c>
       <c r="B23">
         <v>770</v>
       </c>
       <c r="E23" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="13"/>
         <v>{x: 30, y: -60},</v>
       </c>
       <c r="F23">
@@ -670,14 +861,14 @@
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A24" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="12"/>
         <v>{x: 870, y: 780},</v>
       </c>
       <c r="B24">
         <v>840</v>
       </c>
       <c r="E24" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="13"/>
         <v>{x: 30, y: -130},</v>
       </c>
       <c r="F24">
@@ -686,7 +877,7 @@
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A25" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="12"/>
         <v>{x: 940, y: 780},</v>
       </c>
       <c r="B25">
@@ -695,7 +886,7 @@
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A26" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="12"/>
         <v>{x: 1010, y: 780},</v>
       </c>
       <c r="B26">
@@ -704,7 +895,7 @@
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A27" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="12"/>
         <v>{x: 1080, y: 780},</v>
       </c>
       <c r="B27">
@@ -713,7 +904,7 @@
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A28" t="str">
-        <f t="shared" ref="A28:A50" si="2">"{x: "&amp;30+$B28&amp;", y: "&amp;$B$1&amp;"},"</f>
+        <f t="shared" ref="A28:A50" si="18">"{x: "&amp;30+$B28&amp;", y: "&amp;$B$1&amp;"},"</f>
         <v>{x: 1150, y: 780},</v>
       </c>
       <c r="B28">
@@ -722,7 +913,7 @@
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A29" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="18"/>
         <v>{x: 1220, y: 780},</v>
       </c>
       <c r="B29">
@@ -731,7 +922,7 @@
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A30" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="18"/>
         <v>{x: 1290, y: 780},</v>
       </c>
       <c r="B30">
@@ -740,7 +931,7 @@
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A31" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="18"/>
         <v>{x: 1360, y: 780},</v>
       </c>
       <c r="B31">
@@ -749,7 +940,7 @@
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A32" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="18"/>
         <v>{x: 1430, y: 780},</v>
       </c>
       <c r="B32">
@@ -758,7 +949,7 @@
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A33" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="18"/>
         <v>{x: 1500, y: 780},</v>
       </c>
       <c r="B33">
@@ -767,7 +958,7 @@
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A34" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="18"/>
         <v>{x: 1570, y: 780},</v>
       </c>
       <c r="B34">
@@ -776,7 +967,7 @@
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A35" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="18"/>
         <v>{x: 1640, y: 780},</v>
       </c>
       <c r="B35">
@@ -785,7 +976,7 @@
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A36" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="18"/>
         <v>{x: 1710, y: 780},</v>
       </c>
       <c r="B36">
@@ -797,7 +988,7 @@
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A37" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="18"/>
         <v>{x: 1780, y: 780},</v>
       </c>
       <c r="B37">
@@ -806,7 +997,7 @@
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A38" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="18"/>
         <v>{x: 1850, y: 780},</v>
       </c>
       <c r="B38">
@@ -815,7 +1006,7 @@
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A39" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="18"/>
         <v>{x: 1920, y: 780},</v>
       </c>
       <c r="B39">
@@ -824,7 +1015,7 @@
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A40" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="18"/>
         <v>{x: 1990, y: 780},</v>
       </c>
       <c r="B40">
@@ -833,7 +1024,7 @@
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A41" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="18"/>
         <v>{x: 2060, y: 780},</v>
       </c>
       <c r="B41">
@@ -842,7 +1033,7 @@
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A42" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="18"/>
         <v>{x: 2130, y: 780},</v>
       </c>
       <c r="B42">
@@ -851,7 +1042,7 @@
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A43" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="18"/>
         <v>{x: 2200, y: 780},</v>
       </c>
       <c r="B43">
@@ -860,7 +1051,7 @@
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A44" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="18"/>
         <v>{x: 2270, y: 780},</v>
       </c>
       <c r="B44">
@@ -869,7 +1060,7 @@
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A45" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="18"/>
         <v>{x: 2340, y: 780},</v>
       </c>
       <c r="B45">
@@ -878,7 +1069,7 @@
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A46" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="18"/>
         <v>{x: 2410, y: 780},</v>
       </c>
       <c r="B46">
@@ -887,7 +1078,7 @@
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A47" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="18"/>
         <v>{x: 2480, y: 780},</v>
       </c>
       <c r="B47">
@@ -896,74 +1087,518 @@
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A48" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="18"/>
         <v>{x: 2550, y: 780},</v>
       </c>
       <c r="B48">
         <v>2520</v>
       </c>
     </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A49" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="18"/>
         <v>{x: 2620, y: 780},</v>
       </c>
       <c r="B49">
         <v>2590</v>
       </c>
     </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A50" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="18"/>
         <v>{x: 2690, y: 780},</v>
       </c>
       <c r="B50">
         <v>2660</v>
       </c>
     </row>
-    <row r="51" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A51" t="s">
+    <row r="59" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="E59" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="52" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A52" t="s">
+    <row r="60" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="E60" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="53" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A53" t="s">
+    <row r="61" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="E61" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="54" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A54" t="s">
+    <row r="62" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="E62" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="55" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A55" t="s">
+    <row r="63" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="E63" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="56" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A56" t="s">
+    <row r="64" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="E64" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="57" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A57" t="s">
+    <row r="65" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E65" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="58" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A58" t="s">
+    <row r="66" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E66" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="59" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A59" t="s">
+    <row r="67" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E67" t="s">
         <v>18</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{928C9AAB-A0DF-4A28-B539-03523D91F224}">
+  <dimension ref="A1:D73"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="A19" sqref="A19"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="16.2" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="34.77734375" customWidth="1"/>
+    <col min="2" max="2" width="40" customWidth="1"/>
+    <col min="3" max="3" width="26.6640625" customWidth="1"/>
+    <col min="4" max="4" width="22" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B1">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>21</v>
+      </c>
+      <c r="B11" t="s">
+        <v>20</v>
+      </c>
+      <c r="C11" t="s">
+        <v>22</v>
+      </c>
+      <c r="D11" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A12" t="str">
+        <f>"{x: "&amp;0+(ROW()-12)*$B$1&amp;", y: "&amp;780&amp;"},"</f>
+        <v>{x: 0, y: 780},</v>
+      </c>
+      <c r="B12" t="str">
+        <f>"{x: "&amp;1470+(ROW()-12)*$B$1&amp;", y: "&amp;780&amp;"},"</f>
+        <v>{x: 1470, y: 780},</v>
+      </c>
+      <c r="C12" t="s">
+        <v>23</v>
+      </c>
+      <c r="D12" t="str">
+        <f>"{x: "&amp;1680+(ROW()-12)*$B$1&amp;", y: "&amp;500&amp;"},"</f>
+        <v>{x: 1680, y: 500},</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A13" t="str">
+        <f>"{x: "&amp;0+(ROW()-12)*$B$1&amp;", y: "&amp;780&amp;"},"</f>
+        <v>{x: 70, y: 780},</v>
+      </c>
+      <c r="B13" t="str">
+        <f t="shared" ref="B13:B16" si="0">"{x: "&amp;1470+(ROW()-12)*$B$1&amp;", y: "&amp;780&amp;"},"</f>
+        <v>{x: 1540, y: 780},</v>
+      </c>
+      <c r="D13" t="str">
+        <f t="shared" ref="D13:D18" si="1">"{x: "&amp;1680+(ROW()-12)*$B$1&amp;", y: "&amp;500&amp;"},"</f>
+        <v>{x: 1750, y: 500},</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A14" t="str">
+        <f t="shared" ref="A14:A37" si="2">"{x: "&amp;0+(ROW()-12)*$B$1&amp;", y: "&amp;780&amp;"},"</f>
+        <v>{x: 140, y: 780},</v>
+      </c>
+      <c r="B14" t="str">
+        <f t="shared" si="0"/>
+        <v>{x: 1610, y: 780},</v>
+      </c>
+      <c r="D14" t="str">
+        <f t="shared" si="1"/>
+        <v>{x: 1820, y: 500},</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A15" t="str">
+        <f t="shared" si="2"/>
+        <v>{x: 210, y: 780},</v>
+      </c>
+      <c r="B15" t="str">
+        <f t="shared" si="0"/>
+        <v>{x: 1680, y: 780},</v>
+      </c>
+      <c r="D15" t="str">
+        <f t="shared" si="1"/>
+        <v>{x: 1890, y: 500},</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A16" t="str">
+        <f t="shared" si="2"/>
+        <v>{x: 280, y: 780},</v>
+      </c>
+      <c r="B16" t="str">
+        <f t="shared" si="0"/>
+        <v>{x: 1750, y: 780},</v>
+      </c>
+      <c r="D16" t="str">
+        <f t="shared" si="1"/>
+        <v>{x: 1960, y: 500},</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A17" t="str">
+        <f t="shared" si="2"/>
+        <v>{x: 350, y: 780},</v>
+      </c>
+      <c r="D17" t="str">
+        <f t="shared" si="1"/>
+        <v>{x: 2030, y: 500},</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A18" t="str">
+        <f t="shared" si="2"/>
+        <v>{x: 420, y: 780},</v>
+      </c>
+      <c r="D18" t="str">
+        <f>"{x: "&amp;1680+(ROW()-12)*$B$1&amp;", y: "&amp;500&amp;"},"</f>
+        <v>{x: 2100, y: 500},</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A19" t="str">
+        <f>"{x: "&amp;0+(ROW()-12)*$B$1&amp;", y: "&amp;780&amp;"},"</f>
+        <v>{x: 490, y: 780},</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A20" t="str">
+        <f t="shared" si="2"/>
+        <v>{x: 560, y: 780},</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A21" t="str">
+        <f t="shared" si="2"/>
+        <v>{x: 630, y: 780},</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A22" t="str">
+        <f t="shared" si="2"/>
+        <v>{x: 700, y: 780},</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A23" t="str">
+        <f t="shared" si="2"/>
+        <v>{x: 770, y: 780},</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A24" t="str">
+        <f t="shared" si="2"/>
+        <v>{x: 840, y: 780},</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A25" t="str">
+        <f t="shared" si="2"/>
+        <v>{x: 910, y: 780},</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A30" t="str">
+        <f t="shared" si="2"/>
+        <v>{x: 1260, y: 780},</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A31" t="str">
+        <f t="shared" si="2"/>
+        <v>{x: 1330, y: 780},</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A32" t="str">
+        <f t="shared" si="2"/>
+        <v>{x: 1400, y: 780},</v>
+      </c>
+    </row>
+    <row r="33" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A33" t="str">
+        <f t="shared" si="2"/>
+        <v>{x: 1470, y: 780},</v>
+      </c>
+    </row>
+    <row r="34" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A34" t="str">
+        <f t="shared" si="2"/>
+        <v>{x: 1540, y: 780},</v>
+      </c>
+    </row>
+    <row r="35" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A35" t="str">
+        <f t="shared" si="2"/>
+        <v>{x: 1610, y: 780},</v>
+      </c>
+    </row>
+    <row r="36" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A36" t="str">
+        <f t="shared" si="2"/>
+        <v>{x: 1680, y: 780},</v>
+      </c>
+    </row>
+    <row r="37" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A37" t="str">
+        <f t="shared" si="2"/>
+        <v>{x: 1750, y: 780},</v>
+      </c>
+    </row>
+    <row r="38" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A38" t="str">
+        <f>"{x: "&amp;0+(ROW()-12)*$B$1&amp;", y: "&amp;780&amp;"},"</f>
+        <v>{x: 1820, y: 780},</v>
+      </c>
+    </row>
+    <row r="39" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A39" t="str">
+        <f>"{x: "&amp;0+(ROW()-12)*$B$1&amp;", y: "&amp;780&amp;"},"</f>
+        <v>{x: 1890, y: 780},</v>
+      </c>
+    </row>
+    <row r="40" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A40" t="str">
+        <f t="shared" ref="A40:A49" si="3">"{x: "&amp;0+(ROW()-12)*$B$1&amp;", y: "&amp;780&amp;"},"</f>
+        <v>{x: 1960, y: 780},</v>
+      </c>
+    </row>
+    <row r="41" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A41" t="str">
+        <f t="shared" si="3"/>
+        <v>{x: 2030, y: 780},</v>
+      </c>
+    </row>
+    <row r="42" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A42" t="str">
+        <f t="shared" si="3"/>
+        <v>{x: 2100, y: 780},</v>
+      </c>
+    </row>
+    <row r="43" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A43" t="str">
+        <f t="shared" si="3"/>
+        <v>{x: 2170, y: 780},</v>
+      </c>
+    </row>
+    <row r="44" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A44" t="str">
+        <f t="shared" si="3"/>
+        <v>{x: 2240, y: 780},</v>
+      </c>
+    </row>
+    <row r="45" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A45" t="str">
+        <f t="shared" si="3"/>
+        <v>{x: 2310, y: 780},</v>
+      </c>
+    </row>
+    <row r="46" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A46" t="str">
+        <f t="shared" si="3"/>
+        <v>{x: 2380, y: 780},</v>
+      </c>
+    </row>
+    <row r="47" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A47" t="str">
+        <f t="shared" si="3"/>
+        <v>{x: 2450, y: 780},</v>
+      </c>
+    </row>
+    <row r="48" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A48" t="str">
+        <f t="shared" si="3"/>
+        <v>{x: 2520, y: 780},</v>
+      </c>
+    </row>
+    <row r="49" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A49" t="str">
+        <f t="shared" si="3"/>
+        <v>{x: 2590, y: 780},</v>
+      </c>
+    </row>
+    <row r="50" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A50" t="str">
+        <f>"{x: "&amp;0+(ROW()-12)*$B$1&amp;", y: "&amp;780&amp;"},"</f>
+        <v>{x: 2660, y: 780},</v>
+      </c>
+    </row>
+    <row r="51" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A51" t="str">
+        <f>"{x: "&amp;0+(ROW()-12)*$B$1&amp;", y: "&amp;780&amp;"},"</f>
+        <v>{x: 2730, y: 780},</v>
+      </c>
+    </row>
+    <row r="52" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A52" t="str">
+        <f t="shared" ref="A52:A76" si="4">"{x: "&amp;0+(ROW()-12)*$B$1&amp;", y: "&amp;780&amp;"},"</f>
+        <v>{x: 2800, y: 780},</v>
+      </c>
+    </row>
+    <row r="53" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A53" t="str">
+        <f t="shared" si="4"/>
+        <v>{x: 2870, y: 780},</v>
+      </c>
+    </row>
+    <row r="54" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A54" t="str">
+        <f t="shared" si="4"/>
+        <v>{x: 2940, y: 780},</v>
+      </c>
+    </row>
+    <row r="55" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A55" t="str">
+        <f t="shared" si="4"/>
+        <v>{x: 3010, y: 780},</v>
+      </c>
+    </row>
+    <row r="56" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A56" t="str">
+        <f t="shared" si="4"/>
+        <v>{x: 3080, y: 780},</v>
+      </c>
+    </row>
+    <row r="57" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A57" t="str">
+        <f t="shared" si="4"/>
+        <v>{x: 3150, y: 780},</v>
+      </c>
+    </row>
+    <row r="58" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A58" t="str">
+        <f t="shared" si="4"/>
+        <v>{x: 3220, y: 780},</v>
+      </c>
+    </row>
+    <row r="59" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A59" t="str">
+        <f t="shared" si="4"/>
+        <v>{x: 3290, y: 780},</v>
+      </c>
+    </row>
+    <row r="60" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A60" t="str">
+        <f t="shared" si="4"/>
+        <v>{x: 3360, y: 780},</v>
+      </c>
+    </row>
+    <row r="61" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A61" t="str">
+        <f t="shared" si="4"/>
+        <v>{x: 3430, y: 780},</v>
+      </c>
+    </row>
+    <row r="62" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A62" t="str">
+        <f t="shared" si="4"/>
+        <v>{x: 3500, y: 780},</v>
+      </c>
+    </row>
+    <row r="63" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A63" t="str">
+        <f t="shared" si="4"/>
+        <v>{x: 3570, y: 780},</v>
+      </c>
+    </row>
+    <row r="64" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A64" t="str">
+        <f t="shared" si="4"/>
+        <v>{x: 3640, y: 780},</v>
+      </c>
+    </row>
+    <row r="65" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A65" t="str">
+        <f t="shared" si="4"/>
+        <v>{x: 3710, y: 780},</v>
+      </c>
+    </row>
+    <row r="66" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A66" t="str">
+        <f t="shared" si="4"/>
+        <v>{x: 3780, y: 780},</v>
+      </c>
+    </row>
+    <row r="67" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A67" t="str">
+        <f t="shared" si="4"/>
+        <v>{x: 3850, y: 780},</v>
+      </c>
+    </row>
+    <row r="68" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A68" t="str">
+        <f t="shared" si="4"/>
+        <v>{x: 3920, y: 780},</v>
+      </c>
+    </row>
+    <row r="69" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A69" t="str">
+        <f t="shared" si="4"/>
+        <v>{x: 3990, y: 780},</v>
+      </c>
+    </row>
+    <row r="70" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A70" t="str">
+        <f t="shared" si="4"/>
+        <v>{x: 4060, y: 780},</v>
+      </c>
+    </row>
+    <row r="71" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A71" t="str">
+        <f t="shared" si="4"/>
+        <v>{x: 4130, y: 780},</v>
+      </c>
+    </row>
+    <row r="72" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A72" t="str">
+        <f t="shared" si="4"/>
+        <v>{x: 4200, y: 780},</v>
+      </c>
+    </row>
+    <row r="73" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A73" t="str">
+        <f t="shared" si="4"/>
+        <v>{x: 4270, y: 780},</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add monster & collision & update camera & fix Pipe  & update hero img
</commit_message>
<xml_diff>
--- a/coordinate.xlsx
+++ b/coordinate.xlsx
@@ -9,13 +9,13 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="440" windowWidth="16200" windowHeight="10220" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="10220" yWindow="5600" windowWidth="16200" windowHeight="10220" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="工作表1" sheetId="1" r:id="rId1"/>
     <sheet name="工作表2" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="179017" concurrentCalc="0"/>
+  <calcPr calcId="150001" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
@@ -1167,8 +1167,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D73"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A40" workbookViewId="0">
-      <selection activeCell="B49" sqref="B49"/>
+    <sheetView tabSelected="1" topLeftCell="A24" workbookViewId="0">
+      <selection activeCell="B26" sqref="B26:B29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.15"/>
@@ -1234,7 +1234,7 @@
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A14" t="str">
-        <f t="shared" ref="A14:A37" si="2">"{x: "&amp;0+(ROW()-12)*$B$1&amp;", y: "&amp;780&amp;"},"</f>
+        <f t="shared" ref="A14:B37" si="2">"{x: "&amp;0+(ROW()-12)*$B$1&amp;", y: "&amp;780&amp;"},"</f>
         <v>{x: 140, y: 780},</v>
       </c>
       <c r="B14" t="str">
@@ -1334,6 +1334,30 @@
       <c r="A25" t="str">
         <f t="shared" si="2"/>
         <v>{x: 910, y: 780},</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="B26" t="str">
+        <f t="shared" si="2"/>
+        <v>{x: 980, y: 780},</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="B27" t="str">
+        <f t="shared" si="2"/>
+        <v>{x: 1050, y: 780},</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="B28" t="str">
+        <f t="shared" si="2"/>
+        <v>{x: 1120, y: 780},</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="B29" t="str">
+        <f t="shared" si="2"/>
+        <v>{x: 1190, y: 780},</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.15">

</xml_diff>

<commit_message>
Add: fix princess display & map right display
</commit_message>
<xml_diff>
--- a/coordinate.xlsx
+++ b/coordinate.xlsx
@@ -1,22 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19226"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="28410"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\OOP_SuperAdventure\測試\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kelvin/Desktop/OOP_SuperAdventure/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{226584F1-A705-43EA-BB9E-6376DF3C6C1D}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16200" windowHeight="5592" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="10220" yWindow="5600" windowWidth="16200" windowHeight="10220" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="工作表1" sheetId="1" r:id="rId1"/>
     <sheet name="工作表2" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="179017" concurrentCalc="0"/>
+  <calcPr calcId="150001" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
@@ -134,7 +133,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -453,18 +452,18 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L67"/>
   <sheetViews>
-    <sheetView showRuler="0" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C1" sqref="C1:C1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="16.2" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1" width="25.6640625" customWidth="1"/>
-    <col min="5" max="5" width="24.109375" customWidth="1"/>
-    <col min="8" max="8" width="17.109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="24.1640625" customWidth="1"/>
+    <col min="8" max="8" width="17.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.3">
@@ -630,7 +629,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A12" t="str">
         <f>"{x: " &amp; 30+$B12&amp;", y: "&amp;$B$1&amp;"},"</f>
         <v>{x: 30, y: 780},</v>
@@ -661,7 +660,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A13" t="str">
         <f t="shared" ref="A13:A27" si="12">"{x: "&amp;30+$B13&amp;", y: "&amp;$B$1&amp;"},"</f>
         <v>{x: 100, y: 780},</v>
@@ -684,7 +683,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A14" t="str">
         <f t="shared" si="12"/>
         <v>{x: 170, y: 780},</v>
@@ -707,7 +706,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A15" t="str">
         <f t="shared" si="12"/>
         <v>{x: 240, y: 780},</v>
@@ -727,7 +726,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A16" t="str">
         <f t="shared" si="12"/>
         <v>{x: 310, y: 780},</v>
@@ -747,7 +746,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A17" t="str">
         <f t="shared" si="12"/>
         <v>{x: 380, y: 780},</v>
@@ -763,7 +762,7 @@
         <v>350</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A18" t="str">
         <f t="shared" si="12"/>
         <v>{x: 450, y: 780},</v>
@@ -779,7 +778,7 @@
         <v>420</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A19" t="str">
         <f t="shared" si="12"/>
         <v>{x: 520, y: 780},</v>
@@ -795,7 +794,7 @@
         <v>490</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A20" t="str">
         <f t="shared" si="12"/>
         <v>{x: 590, y: 780},</v>
@@ -811,7 +810,7 @@
         <v>560</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A21" t="str">
         <f t="shared" si="12"/>
         <v>{x: 660, y: 780},</v>
@@ -827,7 +826,7 @@
         <v>630</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A22" t="str">
         <f t="shared" si="12"/>
         <v>{x: 730, y: 780},</v>
@@ -843,7 +842,7 @@
         <v>700</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A23" t="str">
         <f t="shared" si="12"/>
         <v>{x: 800, y: 780},</v>
@@ -859,7 +858,7 @@
         <v>770</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A24" t="str">
         <f t="shared" si="12"/>
         <v>{x: 870, y: 780},</v>
@@ -875,7 +874,7 @@
         <v>840</v>
       </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A25" t="str">
         <f t="shared" si="12"/>
         <v>{x: 940, y: 780},</v>
@@ -884,7 +883,7 @@
         <v>910</v>
       </c>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A26" t="str">
         <f t="shared" si="12"/>
         <v>{x: 1010, y: 780},</v>
@@ -893,7 +892,7 @@
         <v>980</v>
       </c>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A27" t="str">
         <f t="shared" si="12"/>
         <v>{x: 1080, y: 780},</v>
@@ -902,7 +901,7 @@
         <v>1050</v>
       </c>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A28" t="str">
         <f t="shared" ref="A28:A50" si="18">"{x: "&amp;30+$B28&amp;", y: "&amp;$B$1&amp;"},"</f>
         <v>{x: 1150, y: 780},</v>
@@ -911,7 +910,7 @@
         <v>1120</v>
       </c>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A29" t="str">
         <f t="shared" si="18"/>
         <v>{x: 1220, y: 780},</v>
@@ -920,7 +919,7 @@
         <v>1190</v>
       </c>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A30" t="str">
         <f t="shared" si="18"/>
         <v>{x: 1290, y: 780},</v>
@@ -929,7 +928,7 @@
         <v>1260</v>
       </c>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A31" t="str">
         <f t="shared" si="18"/>
         <v>{x: 1360, y: 780},</v>
@@ -938,7 +937,7 @@
         <v>1330</v>
       </c>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A32" t="str">
         <f t="shared" si="18"/>
         <v>{x: 1430, y: 780},</v>
@@ -947,7 +946,7 @@
         <v>1400</v>
       </c>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A33" t="str">
         <f t="shared" si="18"/>
         <v>{x: 1500, y: 780},</v>
@@ -956,7 +955,7 @@
         <v>1470</v>
       </c>
     </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A34" t="str">
         <f t="shared" si="18"/>
         <v>{x: 1570, y: 780},</v>
@@ -965,7 +964,7 @@
         <v>1540</v>
       </c>
     </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A35" t="str">
         <f t="shared" si="18"/>
         <v>{x: 1640, y: 780},</v>
@@ -974,7 +973,7 @@
         <v>1610</v>
       </c>
     </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A36" t="str">
         <f t="shared" si="18"/>
         <v>{x: 1710, y: 780},</v>
@@ -986,7 +985,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A37" t="str">
         <f t="shared" si="18"/>
         <v>{x: 1780, y: 780},</v>
@@ -995,7 +994,7 @@
         <v>1750</v>
       </c>
     </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A38" t="str">
         <f t="shared" si="18"/>
         <v>{x: 1850, y: 780},</v>
@@ -1004,7 +1003,7 @@
         <v>1820</v>
       </c>
     </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A39" t="str">
         <f t="shared" si="18"/>
         <v>{x: 1920, y: 780},</v>
@@ -1013,7 +1012,7 @@
         <v>1890</v>
       </c>
     </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A40" t="str">
         <f t="shared" si="18"/>
         <v>{x: 1990, y: 780},</v>
@@ -1022,7 +1021,7 @@
         <v>1960</v>
       </c>
     </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A41" t="str">
         <f t="shared" si="18"/>
         <v>{x: 2060, y: 780},</v>
@@ -1031,7 +1030,7 @@
         <v>2030</v>
       </c>
     </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A42" t="str">
         <f t="shared" si="18"/>
         <v>{x: 2130, y: 780},</v>
@@ -1040,7 +1039,7 @@
         <v>2100</v>
       </c>
     </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A43" t="str">
         <f t="shared" si="18"/>
         <v>{x: 2200, y: 780},</v>
@@ -1049,7 +1048,7 @@
         <v>2170</v>
       </c>
     </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A44" t="str">
         <f t="shared" si="18"/>
         <v>{x: 2270, y: 780},</v>
@@ -1058,7 +1057,7 @@
         <v>2240</v>
       </c>
     </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A45" t="str">
         <f t="shared" si="18"/>
         <v>{x: 2340, y: 780},</v>
@@ -1067,7 +1066,7 @@
         <v>2310</v>
       </c>
     </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A46" t="str">
         <f t="shared" si="18"/>
         <v>{x: 2410, y: 780},</v>
@@ -1076,7 +1075,7 @@
         <v>2380</v>
       </c>
     </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A47" t="str">
         <f t="shared" si="18"/>
         <v>{x: 2480, y: 780},</v>
@@ -1085,7 +1084,7 @@
         <v>2450</v>
       </c>
     </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A48" t="str">
         <f t="shared" si="18"/>
         <v>{x: 2550, y: 780},</v>
@@ -1094,7 +1093,7 @@
         <v>2520</v>
       </c>
     </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A49" t="str">
         <f t="shared" si="18"/>
         <v>{x: 2620, y: 780},</v>
@@ -1103,7 +1102,7 @@
         <v>2590</v>
       </c>
     </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A50" t="str">
         <f t="shared" si="18"/>
         <v>{x: 2690, y: 780},</v>
@@ -1112,47 +1111,47 @@
         <v>2660</v>
       </c>
     </row>
-    <row r="59" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:5" x14ac:dyDescent="0.15">
       <c r="E59" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="60" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:5" x14ac:dyDescent="0.15">
       <c r="E60" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="61" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:5" x14ac:dyDescent="0.15">
       <c r="E61" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="62" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:5" x14ac:dyDescent="0.15">
       <c r="E62" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="63" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:5" x14ac:dyDescent="0.15">
       <c r="E63" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="64" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:5" x14ac:dyDescent="0.15">
       <c r="E64" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="65" spans="5:5" x14ac:dyDescent="0.3">
+    <row r="65" spans="5:5" x14ac:dyDescent="0.15">
       <c r="E65" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="66" spans="5:5" x14ac:dyDescent="0.3">
+    <row r="66" spans="5:5" x14ac:dyDescent="0.15">
       <c r="E66" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="67" spans="5:5" x14ac:dyDescent="0.3">
+    <row r="67" spans="5:5" x14ac:dyDescent="0.15">
       <c r="E67" t="s">
         <v>18</v>
       </c>
@@ -1165,16 +1164,16 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{928C9AAB-A0DF-4A28-B539-03523D91F224}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D73"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="A19" sqref="A19"/>
+    <sheetView tabSelected="1" topLeftCell="A24" workbookViewId="0">
+      <selection activeCell="B26" sqref="B26:B29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.2" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="34.77734375" customWidth="1"/>
+    <col min="1" max="1" width="34.83203125" customWidth="1"/>
     <col min="2" max="2" width="40" customWidth="1"/>
     <col min="3" max="3" width="26.6640625" customWidth="1"/>
     <col min="4" max="4" width="22" customWidth="1"/>
@@ -1229,13 +1228,13 @@
         <v>{x: 1540, y: 780},</v>
       </c>
       <c r="D13" t="str">
-        <f t="shared" ref="D13:D18" si="1">"{x: "&amp;1680+(ROW()-12)*$B$1&amp;", y: "&amp;500&amp;"},"</f>
+        <f t="shared" ref="D13:D17" si="1">"{x: "&amp;1680+(ROW()-12)*$B$1&amp;", y: "&amp;500&amp;"},"</f>
         <v>{x: 1750, y: 500},</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A14" t="str">
-        <f t="shared" ref="A14:A37" si="2">"{x: "&amp;0+(ROW()-12)*$B$1&amp;", y: "&amp;780&amp;"},"</f>
+        <f t="shared" ref="A14:B37" si="2">"{x: "&amp;0+(ROW()-12)*$B$1&amp;", y: "&amp;780&amp;"},"</f>
         <v>{x: 140, y: 780},</v>
       </c>
       <c r="B14" t="str">
@@ -1307,295 +1306,319 @@
         <v>{x: 560, y: 780},</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A21" t="str">
         <f t="shared" si="2"/>
         <v>{x: 630, y: 780},</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A22" t="str">
         <f t="shared" si="2"/>
         <v>{x: 700, y: 780},</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A23" t="str">
         <f t="shared" si="2"/>
         <v>{x: 770, y: 780},</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A24" t="str">
         <f t="shared" si="2"/>
         <v>{x: 840, y: 780},</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A25" t="str">
         <f t="shared" si="2"/>
         <v>{x: 910, y: 780},</v>
       </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="B26" t="str">
+        <f t="shared" si="2"/>
+        <v>{x: 980, y: 780},</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="B27" t="str">
+        <f t="shared" si="2"/>
+        <v>{x: 1050, y: 780},</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="B28" t="str">
+        <f t="shared" si="2"/>
+        <v>{x: 1120, y: 780},</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="B29" t="str">
+        <f t="shared" si="2"/>
+        <v>{x: 1190, y: 780},</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A30" t="str">
         <f t="shared" si="2"/>
         <v>{x: 1260, y: 780},</v>
       </c>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A31" t="str">
         <f t="shared" si="2"/>
         <v>{x: 1330, y: 780},</v>
       </c>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A32" t="str">
         <f t="shared" si="2"/>
         <v>{x: 1400, y: 780},</v>
       </c>
     </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A33" t="str">
         <f t="shared" si="2"/>
         <v>{x: 1470, y: 780},</v>
       </c>
     </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A34" t="str">
         <f t="shared" si="2"/>
         <v>{x: 1540, y: 780},</v>
       </c>
     </row>
-    <row r="35" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A35" t="str">
         <f t="shared" si="2"/>
         <v>{x: 1610, y: 780},</v>
       </c>
     </row>
-    <row r="36" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A36" t="str">
         <f t="shared" si="2"/>
         <v>{x: 1680, y: 780},</v>
       </c>
     </row>
-    <row r="37" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A37" t="str">
         <f t="shared" si="2"/>
         <v>{x: 1750, y: 780},</v>
       </c>
     </row>
-    <row r="38" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A38" t="str">
         <f>"{x: "&amp;0+(ROW()-12)*$B$1&amp;", y: "&amp;780&amp;"},"</f>
         <v>{x: 1820, y: 780},</v>
       </c>
     </row>
-    <row r="39" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A39" t="str">
         <f>"{x: "&amp;0+(ROW()-12)*$B$1&amp;", y: "&amp;780&amp;"},"</f>
         <v>{x: 1890, y: 780},</v>
       </c>
     </row>
-    <row r="40" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A40" t="str">
         <f t="shared" ref="A40:A49" si="3">"{x: "&amp;0+(ROW()-12)*$B$1&amp;", y: "&amp;780&amp;"},"</f>
         <v>{x: 1960, y: 780},</v>
       </c>
     </row>
-    <row r="41" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A41" t="str">
         <f t="shared" si="3"/>
         <v>{x: 2030, y: 780},</v>
       </c>
     </row>
-    <row r="42" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A42" t="str">
         <f t="shared" si="3"/>
         <v>{x: 2100, y: 780},</v>
       </c>
     </row>
-    <row r="43" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A43" t="str">
         <f t="shared" si="3"/>
         <v>{x: 2170, y: 780},</v>
       </c>
     </row>
-    <row r="44" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A44" t="str">
         <f t="shared" si="3"/>
         <v>{x: 2240, y: 780},</v>
       </c>
     </row>
-    <row r="45" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A45" t="str">
         <f t="shared" si="3"/>
         <v>{x: 2310, y: 780},</v>
       </c>
     </row>
-    <row r="46" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A46" t="str">
         <f t="shared" si="3"/>
         <v>{x: 2380, y: 780},</v>
       </c>
     </row>
-    <row r="47" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A47" t="str">
         <f t="shared" si="3"/>
         <v>{x: 2450, y: 780},</v>
       </c>
     </row>
-    <row r="48" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A48" t="str">
         <f t="shared" si="3"/>
         <v>{x: 2520, y: 780},</v>
       </c>
     </row>
-    <row r="49" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A49" t="str">
         <f t="shared" si="3"/>
         <v>{x: 2590, y: 780},</v>
       </c>
     </row>
-    <row r="50" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A50" t="str">
         <f>"{x: "&amp;0+(ROW()-12)*$B$1&amp;", y: "&amp;780&amp;"},"</f>
         <v>{x: 2660, y: 780},</v>
       </c>
     </row>
-    <row r="51" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A51" t="str">
         <f>"{x: "&amp;0+(ROW()-12)*$B$1&amp;", y: "&amp;780&amp;"},"</f>
         <v>{x: 2730, y: 780},</v>
       </c>
     </row>
-    <row r="52" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A52" t="str">
-        <f t="shared" ref="A52:A76" si="4">"{x: "&amp;0+(ROW()-12)*$B$1&amp;", y: "&amp;780&amp;"},"</f>
+        <f t="shared" ref="A52:A73" si="4">"{x: "&amp;0+(ROW()-12)*$B$1&amp;", y: "&amp;780&amp;"},"</f>
         <v>{x: 2800, y: 780},</v>
       </c>
     </row>
-    <row r="53" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A53" t="str">
         <f t="shared" si="4"/>
         <v>{x: 2870, y: 780},</v>
       </c>
     </row>
-    <row r="54" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A54" t="str">
         <f t="shared" si="4"/>
         <v>{x: 2940, y: 780},</v>
       </c>
     </row>
-    <row r="55" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A55" t="str">
         <f t="shared" si="4"/>
         <v>{x: 3010, y: 780},</v>
       </c>
     </row>
-    <row r="56" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A56" t="str">
         <f t="shared" si="4"/>
         <v>{x: 3080, y: 780},</v>
       </c>
     </row>
-    <row r="57" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A57" t="str">
         <f t="shared" si="4"/>
         <v>{x: 3150, y: 780},</v>
       </c>
     </row>
-    <row r="58" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A58" t="str">
         <f t="shared" si="4"/>
         <v>{x: 3220, y: 780},</v>
       </c>
     </row>
-    <row r="59" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A59" t="str">
         <f t="shared" si="4"/>
         <v>{x: 3290, y: 780},</v>
       </c>
     </row>
-    <row r="60" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A60" t="str">
         <f t="shared" si="4"/>
         <v>{x: 3360, y: 780},</v>
       </c>
     </row>
-    <row r="61" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A61" t="str">
         <f t="shared" si="4"/>
         <v>{x: 3430, y: 780},</v>
       </c>
     </row>
-    <row r="62" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A62" t="str">
         <f t="shared" si="4"/>
         <v>{x: 3500, y: 780},</v>
       </c>
     </row>
-    <row r="63" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A63" t="str">
         <f t="shared" si="4"/>
         <v>{x: 3570, y: 780},</v>
       </c>
     </row>
-    <row r="64" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A64" t="str">
         <f t="shared" si="4"/>
         <v>{x: 3640, y: 780},</v>
       </c>
     </row>
-    <row r="65" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A65" t="str">
         <f t="shared" si="4"/>
         <v>{x: 3710, y: 780},</v>
       </c>
     </row>
-    <row r="66" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A66" t="str">
         <f t="shared" si="4"/>
         <v>{x: 3780, y: 780},</v>
       </c>
     </row>
-    <row r="67" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A67" t="str">
         <f t="shared" si="4"/>
         <v>{x: 3850, y: 780},</v>
       </c>
     </row>
-    <row r="68" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A68" t="str">
         <f t="shared" si="4"/>
         <v>{x: 3920, y: 780},</v>
       </c>
     </row>
-    <row r="69" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A69" t="str">
         <f t="shared" si="4"/>
         <v>{x: 3990, y: 780},</v>
       </c>
     </row>
-    <row r="70" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A70" t="str">
         <f t="shared" si="4"/>
         <v>{x: 4060, y: 780},</v>
       </c>
     </row>
-    <row r="71" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A71" t="str">
         <f t="shared" si="4"/>
         <v>{x: 4130, y: 780},</v>
       </c>
     </row>
-    <row r="72" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A72" t="str">
         <f t="shared" si="4"/>
         <v>{x: 4200, y: 780},</v>
       </c>
     </row>
-    <row r="73" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A73" t="str">
         <f t="shared" si="4"/>
         <v>{x: 4270, y: 780},</v>

</xml_diff>

<commit_message>
level1 - fix hero move & hero die
</commit_message>
<xml_diff>
--- a/coordinate.xlsx
+++ b/coordinate.xlsx
@@ -1,22 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19226"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="28410"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\OOP_SuperAdventure\測試\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kelvin/Desktop/OOP_SuperAdventure/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A694AB64-226C-4383-A47D-EF92724DF0C6}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="10224" yWindow="5604" windowWidth="16200" windowHeight="10224" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="10220" yWindow="5600" windowWidth="16200" windowHeight="10220" tabRatio="500" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="工作表1" sheetId="1" r:id="rId1"/>
     <sheet name="工作表2" sheetId="2" r:id="rId2"/>
+    <sheet name="Level1" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="179017" concurrentCalc="0"/>
+  <calcPr calcId="150001" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="49">
   <si>
     <t>gournd_x</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -220,13 +220,17 @@
   </si>
   <si>
     <t>{x: 60, y: 60}</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ground</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -545,21 +549,21 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L67"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C1" sqref="C1:C1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.44140625" defaultRowHeight="16.2" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1" width="25.6640625" customWidth="1"/>
-    <col min="5" max="5" width="24.109375" customWidth="1"/>
-    <col min="8" max="8" width="17.109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="24.1640625" customWidth="1"/>
+    <col min="8" max="8" width="17.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="15" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -567,7 +571,7 @@
         <v>780</v>
       </c>
     </row>
-    <row r="2" spans="1:12" ht="15" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
       <c r="J2">
         <f>I2</f>
         <v>0</v>
@@ -581,7 +585,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:12" ht="15" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
       <c r="J3">
         <f>$I3</f>
         <v>0</v>
@@ -595,7 +599,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:12" ht="15" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
       <c r="J4">
         <f t="shared" ref="J4:J12" si="2">I4</f>
         <v>0</v>
@@ -609,7 +613,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:12" ht="15" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
       <c r="J5">
         <f t="shared" si="2"/>
         <v>0</v>
@@ -623,7 +627,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:12" ht="15" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.3">
       <c r="J6">
         <f t="shared" si="2"/>
         <v>0</v>
@@ -637,7 +641,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:12" ht="15" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.3">
       <c r="J7">
         <f t="shared" si="2"/>
         <v>0</v>
@@ -651,7 +655,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:12" ht="15" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.3">
       <c r="J8">
         <f t="shared" si="2"/>
         <v>0</v>
@@ -665,7 +669,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:12" ht="15" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.3">
       <c r="J9">
         <f t="shared" si="2"/>
         <v>0</v>
@@ -679,7 +683,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:12" ht="15" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.3">
       <c r="J10">
         <f t="shared" si="2"/>
         <v>0</v>
@@ -693,7 +697,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:12" ht="15" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>1</v>
       </c>
@@ -722,7 +726,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A12" t="str">
         <f>"{x: " &amp; 30+$B12&amp;", y: "&amp;$B$1&amp;"},"</f>
         <v>{x: 30, y: 780},</v>
@@ -753,7 +757,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A13" t="str">
         <f t="shared" ref="A13:A27" si="12">"{x: "&amp;30+$B13&amp;", y: "&amp;$B$1&amp;"},"</f>
         <v>{x: 100, y: 780},</v>
@@ -776,7 +780,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A14" t="str">
         <f t="shared" si="12"/>
         <v>{x: 170, y: 780},</v>
@@ -799,7 +803,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A15" t="str">
         <f t="shared" si="12"/>
         <v>{x: 240, y: 780},</v>
@@ -819,7 +823,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A16" t="str">
         <f t="shared" si="12"/>
         <v>{x: 310, y: 780},</v>
@@ -839,7 +843,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A17" t="str">
         <f t="shared" si="12"/>
         <v>{x: 380, y: 780},</v>
@@ -855,7 +859,7 @@
         <v>350</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A18" t="str">
         <f t="shared" si="12"/>
         <v>{x: 450, y: 780},</v>
@@ -871,7 +875,7 @@
         <v>420</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A19" t="str">
         <f t="shared" si="12"/>
         <v>{x: 520, y: 780},</v>
@@ -887,7 +891,7 @@
         <v>490</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A20" t="str">
         <f t="shared" si="12"/>
         <v>{x: 590, y: 780},</v>
@@ -903,7 +907,7 @@
         <v>560</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A21" t="str">
         <f t="shared" si="12"/>
         <v>{x: 660, y: 780},</v>
@@ -919,7 +923,7 @@
         <v>630</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A22" t="str">
         <f t="shared" si="12"/>
         <v>{x: 730, y: 780},</v>
@@ -935,7 +939,7 @@
         <v>700</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A23" t="str">
         <f t="shared" si="12"/>
         <v>{x: 800, y: 780},</v>
@@ -951,7 +955,7 @@
         <v>770</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A24" t="str">
         <f t="shared" si="12"/>
         <v>{x: 870, y: 780},</v>
@@ -967,7 +971,7 @@
         <v>840</v>
       </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A25" t="str">
         <f t="shared" si="12"/>
         <v>{x: 940, y: 780},</v>
@@ -976,7 +980,7 @@
         <v>910</v>
       </c>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A26" t="str">
         <f t="shared" si="12"/>
         <v>{x: 1010, y: 780},</v>
@@ -985,7 +989,7 @@
         <v>980</v>
       </c>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A27" t="str">
         <f t="shared" si="12"/>
         <v>{x: 1080, y: 780},</v>
@@ -994,7 +998,7 @@
         <v>1050</v>
       </c>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A28" t="str">
         <f t="shared" ref="A28:A50" si="18">"{x: "&amp;30+$B28&amp;", y: "&amp;$B$1&amp;"},"</f>
         <v>{x: 1150, y: 780},</v>
@@ -1003,7 +1007,7 @@
         <v>1120</v>
       </c>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A29" t="str">
         <f t="shared" si="18"/>
         <v>{x: 1220, y: 780},</v>
@@ -1012,7 +1016,7 @@
         <v>1190</v>
       </c>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A30" t="str">
         <f t="shared" si="18"/>
         <v>{x: 1290, y: 780},</v>
@@ -1021,7 +1025,7 @@
         <v>1260</v>
       </c>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A31" t="str">
         <f t="shared" si="18"/>
         <v>{x: 1360, y: 780},</v>
@@ -1030,7 +1034,7 @@
         <v>1330</v>
       </c>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A32" t="str">
         <f t="shared" si="18"/>
         <v>{x: 1430, y: 780},</v>
@@ -1039,7 +1043,7 @@
         <v>1400</v>
       </c>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A33" t="str">
         <f t="shared" si="18"/>
         <v>{x: 1500, y: 780},</v>
@@ -1048,7 +1052,7 @@
         <v>1470</v>
       </c>
     </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A34" t="str">
         <f t="shared" si="18"/>
         <v>{x: 1570, y: 780},</v>
@@ -1057,7 +1061,7 @@
         <v>1540</v>
       </c>
     </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A35" t="str">
         <f t="shared" si="18"/>
         <v>{x: 1640, y: 780},</v>
@@ -1066,7 +1070,7 @@
         <v>1610</v>
       </c>
     </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A36" t="str">
         <f t="shared" si="18"/>
         <v>{x: 1710, y: 780},</v>
@@ -1078,7 +1082,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A37" t="str">
         <f t="shared" si="18"/>
         <v>{x: 1780, y: 780},</v>
@@ -1087,7 +1091,7 @@
         <v>1750</v>
       </c>
     </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A38" t="str">
         <f t="shared" si="18"/>
         <v>{x: 1850, y: 780},</v>
@@ -1096,7 +1100,7 @@
         <v>1820</v>
       </c>
     </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A39" t="str">
         <f t="shared" si="18"/>
         <v>{x: 1920, y: 780},</v>
@@ -1105,7 +1109,7 @@
         <v>1890</v>
       </c>
     </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A40" t="str">
         <f t="shared" si="18"/>
         <v>{x: 1990, y: 780},</v>
@@ -1114,7 +1118,7 @@
         <v>1960</v>
       </c>
     </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A41" t="str">
         <f t="shared" si="18"/>
         <v>{x: 2060, y: 780},</v>
@@ -1123,7 +1127,7 @@
         <v>2030</v>
       </c>
     </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A42" t="str">
         <f t="shared" si="18"/>
         <v>{x: 2130, y: 780},</v>
@@ -1132,7 +1136,7 @@
         <v>2100</v>
       </c>
     </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A43" t="str">
         <f t="shared" si="18"/>
         <v>{x: 2200, y: 780},</v>
@@ -1141,7 +1145,7 @@
         <v>2170</v>
       </c>
     </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A44" t="str">
         <f t="shared" si="18"/>
         <v>{x: 2270, y: 780},</v>
@@ -1150,7 +1154,7 @@
         <v>2240</v>
       </c>
     </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A45" t="str">
         <f t="shared" si="18"/>
         <v>{x: 2340, y: 780},</v>
@@ -1159,7 +1163,7 @@
         <v>2310</v>
       </c>
     </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A46" t="str">
         <f t="shared" si="18"/>
         <v>{x: 2410, y: 780},</v>
@@ -1168,7 +1172,7 @@
         <v>2380</v>
       </c>
     </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A47" t="str">
         <f t="shared" si="18"/>
         <v>{x: 2480, y: 780},</v>
@@ -1177,7 +1181,7 @@
         <v>2450</v>
       </c>
     </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A48" t="str">
         <f t="shared" si="18"/>
         <v>{x: 2550, y: 780},</v>
@@ -1186,7 +1190,7 @@
         <v>2520</v>
       </c>
     </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A49" t="str">
         <f t="shared" si="18"/>
         <v>{x: 2620, y: 780},</v>
@@ -1195,7 +1199,7 @@
         <v>2590</v>
       </c>
     </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A50" t="str">
         <f t="shared" si="18"/>
         <v>{x: 2690, y: 780},</v>
@@ -1204,47 +1208,47 @@
         <v>2660</v>
       </c>
     </row>
-    <row r="59" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:5" x14ac:dyDescent="0.15">
       <c r="E59" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="60" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:5" x14ac:dyDescent="0.15">
       <c r="E60" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="61" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:5" x14ac:dyDescent="0.15">
       <c r="E61" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="62" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:5" x14ac:dyDescent="0.15">
       <c r="E62" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="63" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:5" x14ac:dyDescent="0.15">
       <c r="E63" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="64" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:5" x14ac:dyDescent="0.15">
       <c r="E64" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="65" spans="5:5" x14ac:dyDescent="0.3">
+    <row r="65" spans="5:5" x14ac:dyDescent="0.15">
       <c r="E65" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="66" spans="5:5" x14ac:dyDescent="0.3">
+    <row r="66" spans="5:5" x14ac:dyDescent="0.15">
       <c r="E66" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="67" spans="5:5" x14ac:dyDescent="0.3">
+    <row r="67" spans="5:5" x14ac:dyDescent="0.15">
       <c r="E67" t="s">
         <v>18</v>
       </c>
@@ -1257,27 +1261,27 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I73"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G7" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="J11" sqref="J11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="16.2" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1" width="19.6640625" customWidth="1"/>
     <col min="2" max="2" width="27.33203125" customWidth="1"/>
     <col min="3" max="3" width="26.6640625" customWidth="1"/>
     <col min="4" max="4" width="22" customWidth="1"/>
-    <col min="5" max="5" width="16.21875" customWidth="1"/>
-    <col min="6" max="6" width="18.5546875" customWidth="1"/>
-    <col min="7" max="7" width="15.21875" customWidth="1"/>
-    <col min="8" max="8" width="20.21875" customWidth="1"/>
-    <col min="9" max="9" width="12.77734375" customWidth="1"/>
+    <col min="5" max="5" width="16.1640625" customWidth="1"/>
+    <col min="6" max="6" width="18.5" customWidth="1"/>
+    <col min="7" max="7" width="15.1640625" customWidth="1"/>
+    <col min="8" max="8" width="20.1640625" customWidth="1"/>
+    <col min="9" max="9" width="12.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="15" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>19</v>
       </c>
@@ -1285,7 +1289,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="11" spans="1:9" ht="15" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>21</v>
       </c>
@@ -1314,7 +1318,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="12" spans="1:9" ht="15" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A12" t="str">
         <f>"{x: "&amp;0+(ROW()-12)*$B$1&amp;", y: "&amp;780&amp;"},"</f>
         <v>{x: 0, y: 780},</v>
@@ -1346,7 +1350,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A13" t="str">
         <f>"{x: "&amp;0+(ROW()-12)*$B$1&amp;", y: "&amp;780&amp;"},"</f>
         <v>{x: 70, y: 780},</v>
@@ -1359,7 +1363,7 @@
         <v>39</v>
       </c>
       <c r="D13" t="str">
-        <f t="shared" ref="D13:D17" si="1">"{x: "&amp;1680+(ROW()-12)*$B$1&amp;", y: "&amp;500&amp;"},"</f>
+        <f t="shared" ref="D13" si="1">"{x: "&amp;1680+(ROW()-12)*$B$1&amp;", y: "&amp;500&amp;"},"</f>
         <v>{x: 1750, y: 500},</v>
       </c>
       <c r="E13" t="s">
@@ -1369,9 +1373,9 @@
         <v>38</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A14" t="str">
-        <f t="shared" ref="A14:B37" si="2">"{x: "&amp;0+(ROW()-12)*$B$1&amp;", y: "&amp;780&amp;"},"</f>
+        <f t="shared" ref="A14:A37" si="2">"{x: "&amp;0+(ROW()-12)*$B$1&amp;", y: "&amp;780&amp;"},"</f>
         <v>{x: 140, y: 780},</v>
       </c>
       <c r="B14" t="str">
@@ -1388,7 +1392,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A15" t="str">
         <f t="shared" si="2"/>
         <v>{x: 210, y: 780},</v>
@@ -1404,7 +1408,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A16" t="str">
         <f t="shared" si="2"/>
         <v>{x: 280, y: 780},</v>
@@ -1417,7 +1421,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A17" t="str">
         <f t="shared" si="2"/>
         <v>{x: 350, y: 780},</v>
@@ -1426,7 +1430,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A18" t="str">
         <f t="shared" si="2"/>
         <v>{x: 420, y: 780},</v>
@@ -1435,7 +1439,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A19" t="str">
         <f>"{x: "&amp;0+(ROW()-12)*$B$1&amp;", y: "&amp;780&amp;"},"</f>
         <v>{x: 490, y: 780},</v>
@@ -1444,7 +1448,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A20" t="str">
         <f t="shared" si="2"/>
         <v>{x: 560, y: 780},</v>
@@ -1453,7 +1457,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A21" t="str">
         <f t="shared" si="2"/>
         <v>{x: 630, y: 780},</v>
@@ -1462,259 +1466,259 @@
         <v>30</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A22" t="str">
         <f t="shared" si="2"/>
         <v>{x: 700, y: 780},</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A23" t="str">
         <f t="shared" si="2"/>
         <v>{x: 770, y: 780},</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A24" t="str">
         <f t="shared" si="2"/>
         <v>{x: 840, y: 780},</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A25" t="str">
         <f t="shared" si="2"/>
         <v>{x: 910, y: 780},</v>
       </c>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A31" t="str">
         <f t="shared" si="2"/>
         <v>{x: 1330, y: 780},</v>
       </c>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A32" t="str">
         <f t="shared" si="2"/>
         <v>{x: 1400, y: 780},</v>
       </c>
     </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A33" t="str">
         <f t="shared" si="2"/>
         <v>{x: 1470, y: 780},</v>
       </c>
     </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A34" t="str">
         <f t="shared" si="2"/>
         <v>{x: 1540, y: 780},</v>
       </c>
     </row>
-    <row r="35" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A35" t="str">
         <f t="shared" si="2"/>
         <v>{x: 1610, y: 780},</v>
       </c>
     </row>
-    <row r="36" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A36" t="str">
         <f t="shared" si="2"/>
         <v>{x: 1680, y: 780},</v>
       </c>
     </row>
-    <row r="37" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A37" t="str">
         <f t="shared" si="2"/>
         <v>{x: 1750, y: 780},</v>
       </c>
     </row>
-    <row r="38" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A38" t="str">
         <f t="shared" ref="A38:A73" si="3">"{x: "&amp;0+(ROW()-12)*$B$1&amp;", y: "&amp;780&amp;"},"</f>
         <v>{x: 1820, y: 780},</v>
       </c>
     </row>
-    <row r="39" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A39" t="str">
         <f t="shared" si="3"/>
         <v>{x: 1890, y: 780},</v>
       </c>
     </row>
-    <row r="40" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A40" t="str">
         <f t="shared" si="3"/>
         <v>{x: 1960, y: 780},</v>
       </c>
     </row>
-    <row r="41" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A41" t="str">
         <f t="shared" si="3"/>
         <v>{x: 2030, y: 780},</v>
       </c>
     </row>
-    <row r="42" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A42" t="str">
         <f t="shared" si="3"/>
         <v>{x: 2100, y: 780},</v>
       </c>
     </row>
-    <row r="43" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A43" t="str">
         <f t="shared" si="3"/>
         <v>{x: 2170, y: 780},</v>
       </c>
     </row>
-    <row r="44" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A44" t="str">
         <f t="shared" si="3"/>
         <v>{x: 2240, y: 780},</v>
       </c>
     </row>
-    <row r="45" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A45" t="str">
         <f t="shared" si="3"/>
         <v>{x: 2310, y: 780},</v>
       </c>
     </row>
-    <row r="46" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A46" t="str">
         <f t="shared" si="3"/>
         <v>{x: 2380, y: 780},</v>
       </c>
     </row>
-    <row r="47" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A47" t="str">
         <f t="shared" si="3"/>
         <v>{x: 2450, y: 780},</v>
       </c>
     </row>
-    <row r="48" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A48" t="str">
         <f t="shared" si="3"/>
         <v>{x: 2520, y: 780},</v>
       </c>
     </row>
-    <row r="49" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A49" t="str">
         <f t="shared" si="3"/>
         <v>{x: 2590, y: 780},</v>
       </c>
     </row>
-    <row r="50" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A50" t="str">
         <f t="shared" si="3"/>
         <v>{x: 2660, y: 780},</v>
       </c>
     </row>
-    <row r="51" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A51" t="str">
         <f t="shared" si="3"/>
         <v>{x: 2730, y: 780},</v>
       </c>
     </row>
-    <row r="52" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A52" t="str">
         <f t="shared" si="3"/>
         <v>{x: 2800, y: 780},</v>
       </c>
     </row>
-    <row r="53" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A53" t="str">
         <f t="shared" si="3"/>
         <v>{x: 2870, y: 780},</v>
       </c>
     </row>
-    <row r="54" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A54" t="str">
         <f t="shared" si="3"/>
         <v>{x: 2940, y: 780},</v>
       </c>
     </row>
-    <row r="55" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A55" t="str">
         <f t="shared" si="3"/>
         <v>{x: 3010, y: 780},</v>
       </c>
     </row>
-    <row r="56" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A56" t="str">
         <f t="shared" si="3"/>
         <v>{x: 3080, y: 780},</v>
       </c>
     </row>
-    <row r="57" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A57" t="str">
         <f t="shared" si="3"/>
         <v>{x: 3150, y: 780},</v>
       </c>
     </row>
-    <row r="58" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A58" t="str">
         <f t="shared" si="3"/>
         <v>{x: 3220, y: 780},</v>
       </c>
     </row>
-    <row r="59" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A59" t="str">
         <f t="shared" si="3"/>
         <v>{x: 3290, y: 780},</v>
       </c>
     </row>
-    <row r="60" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A60" t="str">
         <f t="shared" si="3"/>
         <v>{x: 3360, y: 780},</v>
       </c>
     </row>
-    <row r="61" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A61" t="str">
         <f t="shared" si="3"/>
         <v>{x: 3430, y: 780},</v>
       </c>
     </row>
-    <row r="62" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A62" t="str">
         <f t="shared" si="3"/>
         <v>{x: 3500, y: 780},</v>
       </c>
     </row>
-    <row r="63" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A63" t="str">
         <f t="shared" si="3"/>
         <v>{x: 3570, y: 780},</v>
       </c>
     </row>
-    <row r="64" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A64" t="str">
         <f t="shared" si="3"/>
         <v>{x: 3640, y: 780},</v>
       </c>
     </row>
-    <row r="69" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A69" t="str">
         <f t="shared" si="3"/>
         <v>{x: 3990, y: 780},</v>
       </c>
     </row>
-    <row r="70" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A70" t="str">
         <f t="shared" si="3"/>
         <v>{x: 4060, y: 780},</v>
       </c>
     </row>
-    <row r="71" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A71" t="str">
         <f t="shared" si="3"/>
         <v>{x: 4130, y: 780},</v>
       </c>
     </row>
-    <row r="72" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A72" t="str">
         <f t="shared" si="3"/>
         <v>{x: 4200, y: 780},</v>
       </c>
     </row>
-    <row r="73" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A73" t="str">
         <f t="shared" si="3"/>
         <v>{x: 4270, y: 780},</v>
@@ -1725,4 +1729,28 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.15"/>
+  <cols>
+    <col min="1" max="1" width="38.5" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A1" t="s">
+        <v>48</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Add: block_Go && cloud_thron
</commit_message>
<xml_diff>
--- a/coordinate.xlsx
+++ b/coordinate.xlsx
@@ -1,22 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="28410"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19226"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kelvin/Desktop/OOP_SuperAdventure/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\OOP_SuperAdventure\測試\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A694AB64-226C-4383-A47D-EF92724DF0C6}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="10220" yWindow="5600" windowWidth="16200" windowHeight="10220" tabRatio="500" activeTab="2"/>
+    <workbookView xWindow="10224" yWindow="5604" windowWidth="16200" windowHeight="10224" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="工作表1" sheetId="1" r:id="rId1"/>
     <sheet name="工作表2" sheetId="2" r:id="rId2"/>
-    <sheet name="Level1" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="150001" concurrentCalc="0"/>
+  <calcPr calcId="179017" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="48">
   <si>
     <t>gournd_x</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -220,17 +220,13 @@
   </si>
   <si>
     <t>{x: 60, y: 60}</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>ground</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -549,21 +545,21 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:L67"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C1" sqref="C1:C1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="11.44140625" defaultRowHeight="16.2" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="25.6640625" customWidth="1"/>
-    <col min="5" max="5" width="24.1640625" customWidth="1"/>
-    <col min="8" max="8" width="17.1640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="24.109375" customWidth="1"/>
+    <col min="8" max="8" width="17.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:12" ht="15" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -571,7 +567,7 @@
         <v>780</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:12" ht="15" x14ac:dyDescent="0.3">
       <c r="J2">
         <f>I2</f>
         <v>0</v>
@@ -585,7 +581,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:12" ht="15" x14ac:dyDescent="0.3">
       <c r="J3">
         <f>$I3</f>
         <v>0</v>
@@ -599,7 +595,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:12" ht="15" x14ac:dyDescent="0.3">
       <c r="J4">
         <f t="shared" ref="J4:J12" si="2">I4</f>
         <v>0</v>
@@ -613,7 +609,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:12" ht="15" x14ac:dyDescent="0.3">
       <c r="J5">
         <f t="shared" si="2"/>
         <v>0</v>
@@ -627,7 +623,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:12" ht="15" x14ac:dyDescent="0.3">
       <c r="J6">
         <f t="shared" si="2"/>
         <v>0</v>
@@ -641,7 +637,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:12" ht="15" x14ac:dyDescent="0.3">
       <c r="J7">
         <f t="shared" si="2"/>
         <v>0</v>
@@ -655,7 +651,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:12" ht="15" x14ac:dyDescent="0.3">
       <c r="J8">
         <f t="shared" si="2"/>
         <v>0</v>
@@ -669,7 +665,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:12" ht="15" x14ac:dyDescent="0.3">
       <c r="J9">
         <f t="shared" si="2"/>
         <v>0</v>
@@ -683,7 +679,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:12" ht="15" x14ac:dyDescent="0.3">
       <c r="J10">
         <f t="shared" si="2"/>
         <v>0</v>
@@ -697,7 +693,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:12" ht="15" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>1</v>
       </c>
@@ -726,7 +722,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A12" t="str">
         <f>"{x: " &amp; 30+$B12&amp;", y: "&amp;$B$1&amp;"},"</f>
         <v>{x: 30, y: 780},</v>
@@ -757,7 +753,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A13" t="str">
         <f t="shared" ref="A13:A27" si="12">"{x: "&amp;30+$B13&amp;", y: "&amp;$B$1&amp;"},"</f>
         <v>{x: 100, y: 780},</v>
@@ -780,7 +776,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A14" t="str">
         <f t="shared" si="12"/>
         <v>{x: 170, y: 780},</v>
@@ -803,7 +799,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.15">
+    <row r="15" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A15" t="str">
         <f t="shared" si="12"/>
         <v>{x: 240, y: 780},</v>
@@ -823,7 +819,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.15">
+    <row r="16" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A16" t="str">
         <f t="shared" si="12"/>
         <v>{x: 310, y: 780},</v>
@@ -843,7 +839,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.15">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A17" t="str">
         <f t="shared" si="12"/>
         <v>{x: 380, y: 780},</v>
@@ -859,7 +855,7 @@
         <v>350</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.15">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A18" t="str">
         <f t="shared" si="12"/>
         <v>{x: 450, y: 780},</v>
@@ -875,7 +871,7 @@
         <v>420</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.15">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A19" t="str">
         <f t="shared" si="12"/>
         <v>{x: 520, y: 780},</v>
@@ -891,7 +887,7 @@
         <v>490</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.15">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A20" t="str">
         <f t="shared" si="12"/>
         <v>{x: 590, y: 780},</v>
@@ -907,7 +903,7 @@
         <v>560</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.15">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A21" t="str">
         <f t="shared" si="12"/>
         <v>{x: 660, y: 780},</v>
@@ -923,7 +919,7 @@
         <v>630</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.15">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A22" t="str">
         <f t="shared" si="12"/>
         <v>{x: 730, y: 780},</v>
@@ -939,7 +935,7 @@
         <v>700</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.15">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A23" t="str">
         <f t="shared" si="12"/>
         <v>{x: 800, y: 780},</v>
@@ -955,7 +951,7 @@
         <v>770</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.15">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A24" t="str">
         <f t="shared" si="12"/>
         <v>{x: 870, y: 780},</v>
@@ -971,7 +967,7 @@
         <v>840</v>
       </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.15">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A25" t="str">
         <f t="shared" si="12"/>
         <v>{x: 940, y: 780},</v>
@@ -980,7 +976,7 @@
         <v>910</v>
       </c>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.15">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A26" t="str">
         <f t="shared" si="12"/>
         <v>{x: 1010, y: 780},</v>
@@ -989,7 +985,7 @@
         <v>980</v>
       </c>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.15">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A27" t="str">
         <f t="shared" si="12"/>
         <v>{x: 1080, y: 780},</v>
@@ -998,7 +994,7 @@
         <v>1050</v>
       </c>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.15">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A28" t="str">
         <f t="shared" ref="A28:A50" si="18">"{x: "&amp;30+$B28&amp;", y: "&amp;$B$1&amp;"},"</f>
         <v>{x: 1150, y: 780},</v>
@@ -1007,7 +1003,7 @@
         <v>1120</v>
       </c>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.15">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A29" t="str">
         <f t="shared" si="18"/>
         <v>{x: 1220, y: 780},</v>
@@ -1016,7 +1012,7 @@
         <v>1190</v>
       </c>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.15">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A30" t="str">
         <f t="shared" si="18"/>
         <v>{x: 1290, y: 780},</v>
@@ -1025,7 +1021,7 @@
         <v>1260</v>
       </c>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.15">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A31" t="str">
         <f t="shared" si="18"/>
         <v>{x: 1360, y: 780},</v>
@@ -1034,7 +1030,7 @@
         <v>1330</v>
       </c>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.15">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A32" t="str">
         <f t="shared" si="18"/>
         <v>{x: 1430, y: 780},</v>
@@ -1043,7 +1039,7 @@
         <v>1400</v>
       </c>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="33" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A33" t="str">
         <f t="shared" si="18"/>
         <v>{x: 1500, y: 780},</v>
@@ -1052,7 +1048,7 @@
         <v>1470</v>
       </c>
     </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="34" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A34" t="str">
         <f t="shared" si="18"/>
         <v>{x: 1570, y: 780},</v>
@@ -1061,7 +1057,7 @@
         <v>1540</v>
       </c>
     </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="35" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A35" t="str">
         <f t="shared" si="18"/>
         <v>{x: 1640, y: 780},</v>
@@ -1070,7 +1066,7 @@
         <v>1610</v>
       </c>
     </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="36" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A36" t="str">
         <f t="shared" si="18"/>
         <v>{x: 1710, y: 780},</v>
@@ -1082,7 +1078,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="37" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A37" t="str">
         <f t="shared" si="18"/>
         <v>{x: 1780, y: 780},</v>
@@ -1091,7 +1087,7 @@
         <v>1750</v>
       </c>
     </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="38" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A38" t="str">
         <f t="shared" si="18"/>
         <v>{x: 1850, y: 780},</v>
@@ -1100,7 +1096,7 @@
         <v>1820</v>
       </c>
     </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="39" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A39" t="str">
         <f t="shared" si="18"/>
         <v>{x: 1920, y: 780},</v>
@@ -1109,7 +1105,7 @@
         <v>1890</v>
       </c>
     </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="40" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A40" t="str">
         <f t="shared" si="18"/>
         <v>{x: 1990, y: 780},</v>
@@ -1118,7 +1114,7 @@
         <v>1960</v>
       </c>
     </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="41" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A41" t="str">
         <f t="shared" si="18"/>
         <v>{x: 2060, y: 780},</v>
@@ -1127,7 +1123,7 @@
         <v>2030</v>
       </c>
     </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="42" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A42" t="str">
         <f t="shared" si="18"/>
         <v>{x: 2130, y: 780},</v>
@@ -1136,7 +1132,7 @@
         <v>2100</v>
       </c>
     </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="43" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A43" t="str">
         <f t="shared" si="18"/>
         <v>{x: 2200, y: 780},</v>
@@ -1145,7 +1141,7 @@
         <v>2170</v>
       </c>
     </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="44" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A44" t="str">
         <f t="shared" si="18"/>
         <v>{x: 2270, y: 780},</v>
@@ -1154,7 +1150,7 @@
         <v>2240</v>
       </c>
     </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="45" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A45" t="str">
         <f t="shared" si="18"/>
         <v>{x: 2340, y: 780},</v>
@@ -1163,7 +1159,7 @@
         <v>2310</v>
       </c>
     </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="46" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A46" t="str">
         <f t="shared" si="18"/>
         <v>{x: 2410, y: 780},</v>
@@ -1172,7 +1168,7 @@
         <v>2380</v>
       </c>
     </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="47" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A47" t="str">
         <f t="shared" si="18"/>
         <v>{x: 2480, y: 780},</v>
@@ -1181,7 +1177,7 @@
         <v>2450</v>
       </c>
     </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="48" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A48" t="str">
         <f t="shared" si="18"/>
         <v>{x: 2550, y: 780},</v>
@@ -1190,7 +1186,7 @@
         <v>2520</v>
       </c>
     </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="49" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A49" t="str">
         <f t="shared" si="18"/>
         <v>{x: 2620, y: 780},</v>
@@ -1199,7 +1195,7 @@
         <v>2590</v>
       </c>
     </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="50" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A50" t="str">
         <f t="shared" si="18"/>
         <v>{x: 2690, y: 780},</v>
@@ -1208,47 +1204,47 @@
         <v>2660</v>
       </c>
     </row>
-    <row r="59" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="59" spans="1:5" x14ac:dyDescent="0.3">
       <c r="E59" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="60" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="60" spans="1:5" x14ac:dyDescent="0.3">
       <c r="E60" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="61" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="61" spans="1:5" x14ac:dyDescent="0.3">
       <c r="E61" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="62" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="62" spans="1:5" x14ac:dyDescent="0.3">
       <c r="E62" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="63" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="63" spans="1:5" x14ac:dyDescent="0.3">
       <c r="E63" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="64" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="64" spans="1:5" x14ac:dyDescent="0.3">
       <c r="E64" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="65" spans="5:5" x14ac:dyDescent="0.15">
+    <row r="65" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E65" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="66" spans="5:5" x14ac:dyDescent="0.15">
+    <row r="66" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E66" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="67" spans="5:5" x14ac:dyDescent="0.15">
+    <row r="67" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E67" t="s">
         <v>18</v>
       </c>
@@ -1261,27 +1257,27 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:I73"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="G7" workbookViewId="0">
       <selection activeCell="J11" sqref="J11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="16.2" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="19.6640625" customWidth="1"/>
     <col min="2" max="2" width="27.33203125" customWidth="1"/>
     <col min="3" max="3" width="26.6640625" customWidth="1"/>
     <col min="4" max="4" width="22" customWidth="1"/>
-    <col min="5" max="5" width="16.1640625" customWidth="1"/>
-    <col min="6" max="6" width="18.5" customWidth="1"/>
-    <col min="7" max="7" width="15.1640625" customWidth="1"/>
-    <col min="8" max="8" width="20.1640625" customWidth="1"/>
-    <col min="9" max="9" width="12.83203125" customWidth="1"/>
+    <col min="5" max="5" width="16.21875" customWidth="1"/>
+    <col min="6" max="6" width="18.5546875" customWidth="1"/>
+    <col min="7" max="7" width="15.21875" customWidth="1"/>
+    <col min="8" max="8" width="20.21875" customWidth="1"/>
+    <col min="9" max="9" width="12.77734375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" ht="15" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>19</v>
       </c>
@@ -1289,7 +1285,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:9" ht="15" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>21</v>
       </c>
@@ -1318,7 +1314,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:9" ht="15" x14ac:dyDescent="0.3">
       <c r="A12" t="str">
         <f>"{x: "&amp;0+(ROW()-12)*$B$1&amp;", y: "&amp;780&amp;"},"</f>
         <v>{x: 0, y: 780},</v>
@@ -1350,7 +1346,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A13" t="str">
         <f>"{x: "&amp;0+(ROW()-12)*$B$1&amp;", y: "&amp;780&amp;"},"</f>
         <v>{x: 70, y: 780},</v>
@@ -1363,7 +1359,7 @@
         <v>39</v>
       </c>
       <c r="D13" t="str">
-        <f t="shared" ref="D13" si="1">"{x: "&amp;1680+(ROW()-12)*$B$1&amp;", y: "&amp;500&amp;"},"</f>
+        <f t="shared" ref="D13:D17" si="1">"{x: "&amp;1680+(ROW()-12)*$B$1&amp;", y: "&amp;500&amp;"},"</f>
         <v>{x: 1750, y: 500},</v>
       </c>
       <c r="E13" t="s">
@@ -1373,9 +1369,9 @@
         <v>38</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A14" t="str">
-        <f t="shared" ref="A14:A37" si="2">"{x: "&amp;0+(ROW()-12)*$B$1&amp;", y: "&amp;780&amp;"},"</f>
+        <f t="shared" ref="A14:B37" si="2">"{x: "&amp;0+(ROW()-12)*$B$1&amp;", y: "&amp;780&amp;"},"</f>
         <v>{x: 140, y: 780},</v>
       </c>
       <c r="B14" t="str">
@@ -1392,7 +1388,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A15" t="str">
         <f t="shared" si="2"/>
         <v>{x: 210, y: 780},</v>
@@ -1408,7 +1404,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A16" t="str">
         <f t="shared" si="2"/>
         <v>{x: 280, y: 780},</v>
@@ -1421,7 +1417,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A17" t="str">
         <f t="shared" si="2"/>
         <v>{x: 350, y: 780},</v>
@@ -1430,7 +1426,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A18" t="str">
         <f t="shared" si="2"/>
         <v>{x: 420, y: 780},</v>
@@ -1439,7 +1435,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A19" t="str">
         <f>"{x: "&amp;0+(ROW()-12)*$B$1&amp;", y: "&amp;780&amp;"},"</f>
         <v>{x: 490, y: 780},</v>
@@ -1448,7 +1444,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A20" t="str">
         <f t="shared" si="2"/>
         <v>{x: 560, y: 780},</v>
@@ -1457,7 +1453,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A21" t="str">
         <f t="shared" si="2"/>
         <v>{x: 630, y: 780},</v>
@@ -1466,259 +1462,259 @@
         <v>30</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A22" t="str">
         <f t="shared" si="2"/>
         <v>{x: 700, y: 780},</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A23" t="str">
         <f t="shared" si="2"/>
         <v>{x: 770, y: 780},</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A24" t="str">
         <f t="shared" si="2"/>
         <v>{x: 840, y: 780},</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A25" t="str">
         <f t="shared" si="2"/>
         <v>{x: 910, y: 780},</v>
       </c>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A31" t="str">
         <f t="shared" si="2"/>
         <v>{x: 1330, y: 780},</v>
       </c>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A32" t="str">
         <f t="shared" si="2"/>
         <v>{x: 1400, y: 780},</v>
       </c>
     </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="33" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A33" t="str">
         <f t="shared" si="2"/>
         <v>{x: 1470, y: 780},</v>
       </c>
     </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="34" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A34" t="str">
         <f t="shared" si="2"/>
         <v>{x: 1540, y: 780},</v>
       </c>
     </row>
-    <row r="35" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="35" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A35" t="str">
         <f t="shared" si="2"/>
         <v>{x: 1610, y: 780},</v>
       </c>
     </row>
-    <row r="36" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="36" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A36" t="str">
         <f t="shared" si="2"/>
         <v>{x: 1680, y: 780},</v>
       </c>
     </row>
-    <row r="37" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="37" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A37" t="str">
         <f t="shared" si="2"/>
         <v>{x: 1750, y: 780},</v>
       </c>
     </row>
-    <row r="38" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="38" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A38" t="str">
         <f t="shared" ref="A38:A73" si="3">"{x: "&amp;0+(ROW()-12)*$B$1&amp;", y: "&amp;780&amp;"},"</f>
         <v>{x: 1820, y: 780},</v>
       </c>
     </row>
-    <row r="39" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="39" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A39" t="str">
         <f t="shared" si="3"/>
         <v>{x: 1890, y: 780},</v>
       </c>
     </row>
-    <row r="40" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="40" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A40" t="str">
         <f t="shared" si="3"/>
         <v>{x: 1960, y: 780},</v>
       </c>
     </row>
-    <row r="41" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="41" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A41" t="str">
         <f t="shared" si="3"/>
         <v>{x: 2030, y: 780},</v>
       </c>
     </row>
-    <row r="42" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="42" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A42" t="str">
         <f t="shared" si="3"/>
         <v>{x: 2100, y: 780},</v>
       </c>
     </row>
-    <row r="43" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="43" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A43" t="str">
         <f t="shared" si="3"/>
         <v>{x: 2170, y: 780},</v>
       </c>
     </row>
-    <row r="44" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="44" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A44" t="str">
         <f t="shared" si="3"/>
         <v>{x: 2240, y: 780},</v>
       </c>
     </row>
-    <row r="45" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="45" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A45" t="str">
         <f t="shared" si="3"/>
         <v>{x: 2310, y: 780},</v>
       </c>
     </row>
-    <row r="46" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="46" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A46" t="str">
         <f t="shared" si="3"/>
         <v>{x: 2380, y: 780},</v>
       </c>
     </row>
-    <row r="47" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="47" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A47" t="str">
         <f t="shared" si="3"/>
         <v>{x: 2450, y: 780},</v>
       </c>
     </row>
-    <row r="48" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="48" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A48" t="str">
         <f t="shared" si="3"/>
         <v>{x: 2520, y: 780},</v>
       </c>
     </row>
-    <row r="49" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="49" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A49" t="str">
         <f t="shared" si="3"/>
         <v>{x: 2590, y: 780},</v>
       </c>
     </row>
-    <row r="50" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="50" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A50" t="str">
         <f t="shared" si="3"/>
         <v>{x: 2660, y: 780},</v>
       </c>
     </row>
-    <row r="51" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="51" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A51" t="str">
         <f t="shared" si="3"/>
         <v>{x: 2730, y: 780},</v>
       </c>
     </row>
-    <row r="52" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="52" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A52" t="str">
         <f t="shared" si="3"/>
         <v>{x: 2800, y: 780},</v>
       </c>
     </row>
-    <row r="53" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="53" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A53" t="str">
         <f t="shared" si="3"/>
         <v>{x: 2870, y: 780},</v>
       </c>
     </row>
-    <row r="54" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="54" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A54" t="str">
         <f t="shared" si="3"/>
         <v>{x: 2940, y: 780},</v>
       </c>
     </row>
-    <row r="55" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="55" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A55" t="str">
         <f t="shared" si="3"/>
         <v>{x: 3010, y: 780},</v>
       </c>
     </row>
-    <row r="56" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="56" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A56" t="str">
         <f t="shared" si="3"/>
         <v>{x: 3080, y: 780},</v>
       </c>
     </row>
-    <row r="57" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="57" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A57" t="str">
         <f t="shared" si="3"/>
         <v>{x: 3150, y: 780},</v>
       </c>
     </row>
-    <row r="58" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="58" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A58" t="str">
         <f t="shared" si="3"/>
         <v>{x: 3220, y: 780},</v>
       </c>
     </row>
-    <row r="59" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="59" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A59" t="str">
         <f t="shared" si="3"/>
         <v>{x: 3290, y: 780},</v>
       </c>
     </row>
-    <row r="60" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="60" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A60" t="str">
         <f t="shared" si="3"/>
         <v>{x: 3360, y: 780},</v>
       </c>
     </row>
-    <row r="61" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="61" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A61" t="str">
         <f t="shared" si="3"/>
         <v>{x: 3430, y: 780},</v>
       </c>
     </row>
-    <row r="62" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="62" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A62" t="str">
         <f t="shared" si="3"/>
         <v>{x: 3500, y: 780},</v>
       </c>
     </row>
-    <row r="63" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="63" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A63" t="str">
         <f t="shared" si="3"/>
         <v>{x: 3570, y: 780},</v>
       </c>
     </row>
-    <row r="64" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="64" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A64" t="str">
         <f t="shared" si="3"/>
         <v>{x: 3640, y: 780},</v>
       </c>
     </row>
-    <row r="69" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="69" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A69" t="str">
         <f t="shared" si="3"/>
         <v>{x: 3990, y: 780},</v>
       </c>
     </row>
-    <row r="70" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="70" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A70" t="str">
         <f t="shared" si="3"/>
         <v>{x: 4060, y: 780},</v>
       </c>
     </row>
-    <row r="71" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="71" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A71" t="str">
         <f t="shared" si="3"/>
         <v>{x: 4130, y: 780},</v>
       </c>
     </row>
-    <row r="72" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="72" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A72" t="str">
         <f t="shared" si="3"/>
         <v>{x: 4200, y: 780},</v>
       </c>
     </row>
-    <row r="73" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="73" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A73" t="str">
         <f t="shared" si="3"/>
         <v>{x: 4270, y: 780},</v>
@@ -1729,28 +1725,4 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.15"/>
-  <cols>
-    <col min="1" max="1" width="38.5" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A1" t="s">
-        <v>48</v>
-      </c>
-    </row>
-  </sheetData>
-  <phoneticPr fontId="1" type="noConversion"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>